<commit_message>
test Push on 16092020
</commit_message>
<xml_diff>
--- a/data/MultipleTestData.xlsx
+++ b/data/MultipleTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="MultipleUsers" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="SubLevelTestData" sheetId="4" r:id="rId5"/>
     <sheet name="paralleltest" sheetId="7" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
+    <sheet name="demoparentlevel" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="209">
   <si>
     <t>Username</t>
   </si>
@@ -620,6 +621,33 @@
   </si>
   <si>
     <t>QMS/OP@RE:</t>
+  </si>
+  <si>
+    <t>Mathew</t>
+  </si>
+  <si>
+    <t>01.QMS</t>
+  </si>
+  <si>
+    <t>02.IMS</t>
+  </si>
+  <si>
+    <t>IMS/0</t>
+  </si>
+  <si>
+    <t>QMS/DC/0</t>
+  </si>
+  <si>
+    <t>03.EMS</t>
+  </si>
+  <si>
+    <t>EMS/0</t>
+  </si>
+  <si>
+    <t>04.Supplier QMS</t>
+  </si>
+  <si>
+    <t>S/QMS/0</t>
   </si>
 </sst>
 </file>
@@ -3308,7 +3336,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3783,7 +3811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
@@ -3811,4 +3839,109 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>